<commit_message>
Completed all 6 Investors
</commit_message>
<xml_diff>
--- a/SeleniumAutomation_Validus/Resources/Batumbu_Data.xlsx
+++ b/SeleniumAutomation_Validus/Resources/Batumbu_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17850" windowHeight="5265" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="18255" windowHeight="5490" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PreCondition" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="185">
   <si>
     <t>Test@123</t>
   </si>
@@ -466,9 +466,6 @@
     <t>Fname</t>
   </si>
   <si>
-    <t>ShareHoldername</t>
-  </si>
-  <si>
     <t>ShareHolder</t>
   </si>
   <si>
@@ -545,6 +542,36 @@
   </si>
   <si>
     <t>indocitizens@batumbu.com</t>
+  </si>
+  <si>
+    <t>International_Institution</t>
+  </si>
+  <si>
+    <t>Champ</t>
+  </si>
+  <si>
+    <t>Surya ShareHolder</t>
+  </si>
+  <si>
+    <t>Indonesian_Business_Entity</t>
+  </si>
+  <si>
+    <t>ShareHoldername`</t>
+  </si>
+  <si>
+    <t>135000</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>investinginternational@batumbu.com</t>
+  </si>
+  <si>
+    <t>990990054</t>
+  </si>
+  <si>
+    <t>MavenBuild</t>
   </si>
 </sst>
 </file>
@@ -1087,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BR10"/>
+  <dimension ref="A1:BR11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,9 +1159,11 @@
     <col min="54" max="54" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="80.7109375" customWidth="1"/>
     <col min="60" max="60" width="24.42578125" customWidth="1"/>
-    <col min="63" max="63" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="15.42578125" customWidth="1"/>
-    <col min="68" max="68" width="24.42578125" customWidth="1"/>
+    <col min="62" max="62" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="15.42578125" customWidth="1"/>
+    <col min="65" max="65" width="14.42578125" customWidth="1"/>
+    <col min="66" max="66" width="18.28515625" customWidth="1"/>
+    <col min="67" max="67" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:70" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1241,10 +1270,10 @@
         <v>43</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>44</v>
@@ -1318,37 +1347,37 @@
       <c r="BH1" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="BI1" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="BJ1" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="BL1" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="BM1" s="1" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="BN1" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="BP1" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:70" s="5" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>178</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>134</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>0</v>
@@ -1357,19 +1386,19 @@
         <v>0</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>104</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>1</v>
@@ -1444,10 +1473,10 @@
         <v>8</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AJ2" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AK2" s="5" t="s">
         <v>1</v>
@@ -1462,16 +1491,16 @@
         <v>1</v>
       </c>
       <c r="AO2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP2" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="AP2" s="4" t="s">
-        <v>168</v>
-      </c>
       <c r="AQ2" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AR2" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AS2" s="5" t="s">
         <v>1</v>
@@ -1512,22 +1541,37 @@
       <c r="BH2" s="13" t="s">
         <v>122</v>
       </c>
+      <c r="BI2" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BJ2" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="BK2" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BP2" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BL2" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="BM2" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="BN2" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="BO2" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:70" s="5" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:70" s="5" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>134</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>0</v>
@@ -1536,19 +1580,19 @@
         <v>0</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>66</v>
+        <v>173</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>1</v>
@@ -1563,10 +1607,10 @@
         <v>1</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>166</v>
+        <v>68</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>70</v>
@@ -1593,10 +1637,10 @@
         <v>73</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="AA3" s="7" t="s">
         <v>75</v>
@@ -1623,10 +1667,10 @@
         <v>8</v>
       </c>
       <c r="AI3" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AK3" s="5" t="s">
         <v>1</v>
@@ -1641,16 +1685,16 @@
         <v>1</v>
       </c>
       <c r="AO3" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP3" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="AP3" s="4" t="s">
-        <v>168</v>
-      </c>
       <c r="AQ3" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AR3" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AS3" s="5" t="s">
         <v>1</v>
@@ -1688,43 +1732,61 @@
       <c r="BD3" s="5">
         <v>35</v>
       </c>
-      <c r="BK3" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="BP3" s="4" t="s">
+      <c r="BH3" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="BI3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BJ3" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BK3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BL3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="BM3" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="BN3" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="BO3" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:70" s="5" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:70" s="5" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>134</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>66</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>1</v>
@@ -1733,22 +1795,22 @@
         <v>125</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>109</v>
+        <v>67</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="P4" s="12">
-        <v>41193</v>
+        <v>165</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="S4" s="5" t="s">
         <v>71</v>
@@ -1769,10 +1831,10 @@
         <v>73</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AA4" s="7" t="s">
         <v>75</v>
@@ -1787,7 +1849,7 @@
         <v>126</v>
       </c>
       <c r="AE4" s="5" t="s">
-        <v>162</v>
+        <v>6</v>
       </c>
       <c r="AF4" s="5" t="s">
         <v>7</v>
@@ -1799,10 +1861,10 @@
         <v>8</v>
       </c>
       <c r="AI4" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AJ4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AK4" s="5" t="s">
         <v>1</v>
@@ -1817,16 +1879,16 @@
         <v>1</v>
       </c>
       <c r="AO4" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP4" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="AP4" s="4" t="s">
-        <v>168</v>
-      </c>
       <c r="AQ4" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AR4" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AS4" s="5" t="s">
         <v>1</v>
@@ -1864,22 +1926,40 @@
       <c r="BD4" s="5">
         <v>35</v>
       </c>
-      <c r="BK4" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="BP4" s="4" t="s">
+      <c r="BH4" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="BI4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BJ4" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="BK4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BL4" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="BM4" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="BN4" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="BO4" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:70" s="5" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>134</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>0</v>
@@ -1888,19 +1968,19 @@
         <v>0</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>66</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>107</v>
+        <v>159</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>1</v>
@@ -1909,13 +1989,13 @@
         <v>125</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>117</v>
+        <v>160</v>
       </c>
       <c r="P5" s="12">
         <v>41193</v>
@@ -1963,7 +2043,7 @@
         <v>126</v>
       </c>
       <c r="AE5" s="5" t="s">
-        <v>106</v>
+        <v>161</v>
       </c>
       <c r="AF5" s="5" t="s">
         <v>7</v>
@@ -1975,10 +2055,10 @@
         <v>8</v>
       </c>
       <c r="AI5" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AJ5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AK5" s="5" t="s">
         <v>1</v>
@@ -1993,16 +2073,16 @@
         <v>1</v>
       </c>
       <c r="AO5" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP5" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="AP5" s="4" t="s">
+      <c r="AQ5" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AR5" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="AQ5" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="AR5" s="4" t="s">
-        <v>170</v>
       </c>
       <c r="AS5" s="5" t="s">
         <v>1</v>
@@ -2040,22 +2120,40 @@
       <c r="BD5" s="5">
         <v>35</v>
       </c>
-      <c r="BK5" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="BP5" s="4" t="s">
+      <c r="BH5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="BI5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BJ5" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="BK5" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BL5" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="BM5" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="BN5" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="BO5" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:70" s="5" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>134</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>0</v>
@@ -2064,19 +2162,19 @@
         <v>0</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>66</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>1</v>
@@ -2091,7 +2189,7 @@
         <v>1</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="P6" s="12">
         <v>41193</v>
@@ -2151,10 +2249,10 @@
         <v>8</v>
       </c>
       <c r="AI6" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AJ6" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AK6" s="5" t="s">
         <v>1</v>
@@ -2169,16 +2267,16 @@
         <v>1</v>
       </c>
       <c r="AO6" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP6" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="AP6" s="4" t="s">
-        <v>168</v>
-      </c>
       <c r="AQ6" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AR6" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AS6" s="5" t="s">
         <v>1</v>
@@ -2213,301 +2311,714 @@
       <c r="BC6" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="BD6" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="BE6" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="BF6" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="BG6" s="5" t="s">
-        <v>115</v>
+      <c r="BD6" s="5">
+        <v>35</v>
       </c>
       <c r="BH6" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="BJ6" s="4" t="s">
+      <c r="BI6" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="BK6" s="12">
+      <c r="BJ6" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="BK6" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BL6" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="BM6" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="BN6" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="BO6" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:70" s="5" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="P7" s="12">
+        <v>41193</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD7" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE7" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI7" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="AJ7" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO7" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP7" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="AQ7" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AR7" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="AS7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="BC7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BD7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="BE7" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="BF7" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="BG7" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="BH7" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="BI7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BJ7" s="12">
         <v>42957</v>
       </c>
-      <c r="BP6" s="4" t="s">
-        <v>154</v>
+      <c r="BK7" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BL7" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="BM7" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="BN7" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="BO7" s="4" t="s">
+        <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:70" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AI7" t="s">
+    <row r="8" spans="1:70" s="5" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="P8" s="12">
+        <v>41193</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="W8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y8" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA8" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE8" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI8" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="AJ8" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO8" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP8" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="AQ8" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AR8" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="AS8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="BC8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BD8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="BE8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="BF8" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="BG8" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="BH8" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="BI8" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BJ8" s="12">
+        <v>42957</v>
+      </c>
+      <c r="BK8" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BL8" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="BM8" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="BN8" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="BO8" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="AJ7" t="s">
-        <v>150</v>
-      </c>
     </row>
-    <row r="8" spans="1:70" ht="46.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:70" s="5" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:70" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:70" s="5" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B10" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H10" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="K9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" s="4" t="s">
+      <c r="K10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M10" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="N9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O9" s="5" t="s">
+      <c r="N10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O10" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="P9" s="12">
+      <c r="P10" s="12">
         <v>41193</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="R9" s="5" t="s">
+      <c r="R10" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="S9" s="5" t="s">
+      <c r="S10" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="T9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="U9" s="5" t="s">
+      <c r="T10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U10" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="V9" s="4" t="s">
+      <c r="V10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="W9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="X9" s="4" t="s">
+      <c r="W10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X10" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="Y9" s="5" t="s">
+      <c r="Y10" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="Z9" s="6" t="s">
+      <c r="Z10" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="AA9" s="7" t="s">
+      <c r="AA10" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="AB9" s="4" t="s">
+      <c r="AB10" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AC9" s="5" t="s">
+      <c r="AC10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AD9" s="5" t="s">
+      <c r="AD10" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="AE9" s="5" t="s">
+      <c r="AE10" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="AF9" s="5" t="s">
+      <c r="AF10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AG9" s="4" t="s">
+      <c r="AG10" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AH9" s="5" t="s">
+      <c r="AH10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AK9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO9" s="5">
+      <c r="AK10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO10" s="5">
         <v>10000</v>
       </c>
-      <c r="AP9" s="5">
+      <c r="AP10" s="5">
         <v>1000</v>
       </c>
-      <c r="AQ9" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="AR9" s="5">
+      <c r="AQ10" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AR10" s="5">
         <v>25000</v>
       </c>
-      <c r="AS9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AT9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AU9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AV9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AW9" s="5" t="s">
+      <c r="AS10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AX9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AY9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="BA9" s="5" t="s">
+      <c r="AX10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="BB9" s="5" t="s">
+      <c r="BB10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="BC9" s="5" t="s">
+      <c r="BC10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="BD9" s="4" t="s">
+      <c r="BD10" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="BE9" s="4" t="s">
+      <c r="BE10" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="BF9" s="5" t="s">
+      <c r="BF10" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="BG9" s="5" t="s">
+      <c r="BG10" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="BH9" s="5" t="s">
+      <c r="BH10" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="BJ9" s="5">
+      <c r="BI10" s="5">
         <v>2</v>
       </c>
-      <c r="BK9" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="BL9" s="4" t="s">
+      <c r="BJ10" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="BK10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="BM9" s="4" t="s">
+      <c r="BL10" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="BN9" s="5" t="s">
+      <c r="BM10" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="BO9" s="5" t="s">
+      <c r="BN10" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="BP9" s="5" t="s">
+      <c r="BO10" s="5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:70" s="5" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="3"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="4"/>
-      <c r="AG10" s="4"/>
+    <row r="11" spans="1:70" s="5" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="3"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="4"/>
+      <c r="AG11" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="I2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="H2" r:id="rId5"/>
-    <hyperlink ref="B2" r:id="rId6"/>
-    <hyperlink ref="D3" r:id="rId7"/>
-    <hyperlink ref="E3" r:id="rId8"/>
-    <hyperlink ref="I3" r:id="rId9"/>
-    <hyperlink ref="C3" r:id="rId10"/>
-    <hyperlink ref="H3" r:id="rId11"/>
-    <hyperlink ref="B3" r:id="rId12"/>
-    <hyperlink ref="D4" r:id="rId13"/>
-    <hyperlink ref="E4" r:id="rId14"/>
-    <hyperlink ref="I4" r:id="rId15"/>
-    <hyperlink ref="C4" r:id="rId16"/>
-    <hyperlink ref="H4" r:id="rId17"/>
-    <hyperlink ref="B4" r:id="rId18"/>
-    <hyperlink ref="D5" r:id="rId19"/>
-    <hyperlink ref="E5" r:id="rId20"/>
-    <hyperlink ref="I5" r:id="rId21"/>
-    <hyperlink ref="C5" r:id="rId22"/>
-    <hyperlink ref="H5" r:id="rId23"/>
-    <hyperlink ref="B5" r:id="rId24"/>
-    <hyperlink ref="D6" r:id="rId25"/>
-    <hyperlink ref="E6" r:id="rId26"/>
-    <hyperlink ref="I6" r:id="rId27"/>
-    <hyperlink ref="C6" r:id="rId28"/>
-    <hyperlink ref="H6" r:id="rId29"/>
-    <hyperlink ref="B6" r:id="rId30"/>
-    <hyperlink ref="D9" r:id="rId31"/>
-    <hyperlink ref="E9" r:id="rId32"/>
-    <hyperlink ref="I9" r:id="rId33"/>
-    <hyperlink ref="C9" r:id="rId34"/>
-    <hyperlink ref="H9" r:id="rId35"/>
-    <hyperlink ref="B9" r:id="rId36"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="I3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="H3" r:id="rId5"/>
+    <hyperlink ref="B3" r:id="rId6"/>
+    <hyperlink ref="D4" r:id="rId7"/>
+    <hyperlink ref="E4" r:id="rId8"/>
+    <hyperlink ref="I4" r:id="rId9"/>
+    <hyperlink ref="C4" r:id="rId10"/>
+    <hyperlink ref="H4" r:id="rId11"/>
+    <hyperlink ref="B4" r:id="rId12"/>
+    <hyperlink ref="D5" r:id="rId13"/>
+    <hyperlink ref="E5" r:id="rId14"/>
+    <hyperlink ref="I5" r:id="rId15"/>
+    <hyperlink ref="C5" r:id="rId16"/>
+    <hyperlink ref="H5" r:id="rId17"/>
+    <hyperlink ref="B5" r:id="rId18"/>
+    <hyperlink ref="D6" r:id="rId19"/>
+    <hyperlink ref="E6" r:id="rId20"/>
+    <hyperlink ref="I6" r:id="rId21"/>
+    <hyperlink ref="C6" r:id="rId22"/>
+    <hyperlink ref="H6" r:id="rId23"/>
+    <hyperlink ref="B6" r:id="rId24"/>
+    <hyperlink ref="D7" r:id="rId25"/>
+    <hyperlink ref="E7" r:id="rId26"/>
+    <hyperlink ref="I7" r:id="rId27"/>
+    <hyperlink ref="C7" r:id="rId28"/>
+    <hyperlink ref="H7" r:id="rId29"/>
+    <hyperlink ref="B7" r:id="rId30"/>
+    <hyperlink ref="D10" r:id="rId31"/>
+    <hyperlink ref="E10" r:id="rId32"/>
+    <hyperlink ref="I10" r:id="rId33"/>
+    <hyperlink ref="C10" r:id="rId34"/>
+    <hyperlink ref="H10" r:id="rId35"/>
+    <hyperlink ref="B10" r:id="rId36"/>
+    <hyperlink ref="D8" r:id="rId37"/>
+    <hyperlink ref="E8" r:id="rId38"/>
+    <hyperlink ref="I8" r:id="rId39"/>
+    <hyperlink ref="C8" r:id="rId40"/>
+    <hyperlink ref="H8" r:id="rId41"/>
+    <hyperlink ref="B8" r:id="rId42"/>
+    <hyperlink ref="D2" r:id="rId43"/>
+    <hyperlink ref="E2" r:id="rId44"/>
+    <hyperlink ref="I2" r:id="rId45"/>
+    <hyperlink ref="C2" r:id="rId46"/>
+    <hyperlink ref="H2" r:id="rId47"/>
+    <hyperlink ref="B2" r:id="rId48"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId37"/>
+  <pageSetup orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
 

</xml_diff>